<commit_message>
added product_catalog update function
</commit_message>
<xml_diff>
--- a/prep_and_checklists/Test/PREPLIST_Test_07-05-2025_4.xlsx
+++ b/prep_and_checklists/Test/PREPLIST_Test_07-05-2025_4.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcuvin/purveyor_project/prep_and_checklists/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D82262-BD85-1B46-A5B8-E5278CC6A797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02834DE4-AFB3-0D40-B0AC-BB28FDB53AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prep_sheet" sheetId="1" r:id="rId1"/>
     <sheet name="order_sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="154">
   <si>
     <t>Test 40 Guests 5:30 PM - 7:30 PM Wednesday, July 9, 2025</t>
   </si>
@@ -480,6 +493,9 @@
   </si>
   <si>
     <t>N/a</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -939,7 +955,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -949,6 +965,7 @@
     <col min="8" max="8" width="25.1640625" customWidth="1"/>
     <col min="10" max="10" width="31.33203125" customWidth="1"/>
     <col min="13" max="13" width="19.83203125" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
@@ -1096,6 +1113,9 @@
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="C7" t="s">
+        <v>153</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1561,18 +1581,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>